<commit_message>
Creating a game takes you to the color select window
</commit_message>
<xml_diff>
--- a/Bugs from Phase 2.xlsx
+++ b/Bugs from Phase 2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Number</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>If you login as a player other than the player whose turn it is or the player that immediately finished their turn and rejoin a game, chat will not receive their messages.</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>You can buy dev cards even after there are none left</t>
   </si>
 </sst>
 </file>
@@ -134,10 +140,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,196 +425,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="76.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="76.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>325</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>324</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>322</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>317</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>316</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>315</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>314</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>312</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>311</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>310</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>289</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>287</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>284</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>283</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>196</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>194</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>193</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>191</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>188</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>186</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>185</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel Bug Assignements
</commit_message>
<xml_diff>
--- a/Bugs from Phase 2.xlsx
+++ b/Bugs from Phase 2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Number</t>
   </si>
@@ -98,10 +98,25 @@
     <t>If you login as a player other than the player whose turn it is or the player that immediately finished their turn and rejoin a game, chat will not receive their messages.</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>You can buy dev cards even after there are none left</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Ask Tas</t>
+  </si>
+  <si>
+    <t>Grant</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Justin</t>
   </si>
 </sst>
 </file>
@@ -427,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,6 +471,9 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -464,6 +482,9 @@
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -472,6 +493,9 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -480,6 +504,9 @@
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -488,6 +515,9 @@
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -496,6 +526,9 @@
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -504,6 +537,9 @@
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -512,6 +548,9 @@
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -520,6 +559,9 @@
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -528,6 +570,9 @@
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -536,6 +581,9 @@
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -544,6 +592,9 @@
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -552,6 +603,9 @@
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -561,7 +615,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -571,61 +625,85 @@
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>194</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>193</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>191</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>188</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>186</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>185</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>-1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Once Color is picked, you can't change it
</commit_message>
<xml_diff>
--- a/Bugs from Phase 2.xlsx
+++ b/Bugs from Phase 2.xlsx
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +560,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -582,7 +582,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -615,7 +615,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">

</xml_diff>